<commit_message>
adding ability to find legal pairs
</commit_message>
<xml_diff>
--- a/data/mock_headers.xlsx
+++ b/data/mock_headers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harid\Documents\Spring 2022\SCIJPartnerMatching\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2278C7-9D9E-4BDB-A27A-A6DCC9B23C71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{568E77D5-1B31-46C9-B3F1-4D618170CFF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>header</t>
   </si>
@@ -36,9 +36,6 @@
     <t>necessary</t>
   </si>
   <si>
-    <t>similar_match</t>
-  </si>
-  <si>
     <t>Monday</t>
   </si>
   <si>
@@ -54,10 +51,10 @@
     <t>School</t>
   </si>
   <si>
-    <t>category_one</t>
-  </si>
-  <si>
     <t>hours</t>
+  </si>
+  <si>
+    <t>similar_category_one</t>
   </si>
 </sst>
 </file>
@@ -375,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -387,7 +384,7 @@
     <col min="2" max="2" width="48.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -397,63 +394,48 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding new data and integrating
</commit_message>
<xml_diff>
--- a/data/mock_headers.xlsx
+++ b/data/mock_headers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harid\Documents\Spring 2022\SCIJPartnerMatching\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{568E77D5-1B31-46C9-B3F1-4D618170CFF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8608FDD-1275-41F8-A800-24DA10AEB738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -375,7 +375,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>